<commit_message>
Removed log in pages and deleted unused code
</commit_message>
<xml_diff>
--- a/src/test/resources/Excel/TestData.xlsx
+++ b/src/test/resources/Excel/TestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1332eb67554a452f/Documents/DsAlgoTestNG/src/test/resources/Excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\DsAlgoTestNG-Sru\src\test\resources\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:801_{1F455E17-C5B2-46FA-B26D-55A03271BA7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E216375F-7FCA-45CD-9D9B-62F173303237}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CED9344B-AEBE-4000-B3BF-26B5C228B407}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{01914433-B6EF-45F7-9669-75209D66C2C6}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" activeTab="6" xr2:uid="{01914433-B6EF-45F7-9669-75209D66C2C6}"/>
   </bookViews>
   <sheets>
     <sheet name="python DS" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,10 @@
     <sheet name="Register" sheetId="4" r:id="rId4"/>
     <sheet name="LinkedList" sheetId="5" r:id="rId5"/>
     <sheet name="LoginValidData" sheetId="6" r:id="rId6"/>
+    <sheet name="SearchArray" sheetId="7" r:id="rId7"/>
+    <sheet name="MaxConsecutive" sheetId="8" r:id="rId8"/>
+    <sheet name="FindEventNum" sheetId="9" r:id="rId9"/>
+    <sheet name="SquareSorted" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -30,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="33">
   <si>
     <t>Code</t>
   </si>
@@ -592,14 +596,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F542CB85-55EF-446C-96FE-6338DCB949D1}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="16.3828125" customWidth="1"/>
-    <col min="2" max="2" width="43.3828125" customWidth="1"/>
+    <col min="1" max="1" width="16.4609375" customWidth="1"/>
+    <col min="2" max="2" width="43.4609375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.4">
@@ -614,7 +618,7 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>32</v>
       </c>
     </row>
@@ -622,8 +626,43 @@
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD799DC1-36EF-4DAB-9021-32A3904FC6FB}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A2:XFD3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="227.4609375" customWidth="1"/>
+    <col min="2" max="2" width="33.53515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -636,12 +675,12 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="118.3828125" customWidth="1"/>
+    <col min="1" max="1" width="227.4609375" customWidth="1"/>
     <col min="2" max="2" width="33.53515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -717,8 +756,8 @@
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="18.15234375" customWidth="1"/>
-    <col min="2" max="2" width="16.3046875" customWidth="1"/>
-    <col min="3" max="3" width="30.3828125" customWidth="1"/>
+    <col min="2" max="2" width="16.23046875" customWidth="1"/>
+    <col min="3" max="3" width="30.4609375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.4">
@@ -820,7 +859,7 @@
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="15.84375" customWidth="1"/>
-    <col min="2" max="2" width="18.3828125" customWidth="1"/>
+    <col min="2" max="2" width="18.4609375" customWidth="1"/>
     <col min="3" max="3" width="15.53515625" customWidth="1"/>
     <col min="4" max="4" width="56.53515625" customWidth="1"/>
   </cols>
@@ -990,14 +1029,18 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4F8939E-08F6-4761-981C-885093E6F4D2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1821E0E6-2D89-4C70-BB13-B2E19C8B4D3B}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="16.15234375" customWidth="1"/>
+    <col min="2" max="2" width="26" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
@@ -1017,8 +1060,131 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{3EFF30CB-6268-4D9D-854D-D034E19199E3}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{61EFDAFC-A678-489E-B4EA-1225521BA180}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90497AF2-E708-4EF8-88BC-44CC3E058358}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="227.4609375" customWidth="1"/>
+    <col min="2" max="2" width="33.53515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A3" s="2"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A4" s="2"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A5" s="2"/>
+      <c r="B5" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E628353C-0FB5-4C6B-A5B8-33B4399CEF75}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="227.4609375" customWidth="1"/>
+    <col min="2" max="2" width="33.53515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.600000000000001" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="2"/>
+      <c r="B3" s="1"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A4" s="2"/>
+      <c r="B4" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{426FD891-1E44-41A3-837D-774F075EB1D0}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="227.4609375" customWidth="1"/>
+    <col min="2" max="2" width="33.53515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>